<commit_message>
Online validation of expansion expressions and check function call names
* Online validation of field values where an expansion expression is used
* Check function names when evaluating expressions. The name must be declared in the dictionary "global_functions".
* Assign "default" as system of a Processor if the field "System" is not defined
</commit_message>
<xml_diff>
--- a/backend_tests/z_input_files/v2/18_dataset_expansion_2.xlsx
+++ b/backend_tests/z_input_files/v2/18_dataset_expansion_2.xlsx
@@ -5,13 +5,13 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="1"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="InterfaceTypes" sheetId="1" state="visible" r:id="rId2"/>
-    <sheet name="DatasetDef" sheetId="2" state="visible" r:id="rId3"/>
-    <sheet name="DatasetData TheData" sheetId="3" state="visible" r:id="rId4"/>
-    <sheet name="BareProcessors" sheetId="4" state="visible" r:id="rId5"/>
+    <sheet name="BareProcessors" sheetId="2" state="visible" r:id="rId3"/>
+    <sheet name="DatasetDef" sheetId="3" state="visible" r:id="rId4"/>
+    <sheet name="DatasetData TheData" sheetId="4" state="visible" r:id="rId5"/>
     <sheet name="Interfaces" sheetId="5" state="visible" r:id="rId6"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
@@ -77,6 +77,48 @@
     <t xml:space="preserve">0200</t>
   </si>
   <si>
+    <t xml:space="preserve">ProcessorGroup</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Processor</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ParentProcessor</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SubsystemType</t>
+  </si>
+  <si>
+    <t xml:space="preserve">System</t>
+  </si>
+  <si>
+    <t xml:space="preserve">FunctionalOrStructural</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Accounted</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Stock</t>
+  </si>
+  <si>
+    <t xml:space="preserve">GeolocationRef</t>
+  </si>
+  <si>
+    <t xml:space="preserve">GeolocationCode</t>
+  </si>
+  <si>
+    <t xml:space="preserve">GeolocationLatLong</t>
+  </si>
+  <si>
+    <t xml:space="preserve">p1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">yes</t>
+  </si>
+  <si>
+    <t xml:space="preserve">p2</t>
+  </si>
+  <si>
     <t xml:space="preserve">Dataset</t>
   </si>
   <si>
@@ -123,48 +165,6 @@
   </si>
   <si>
     <t xml:space="preserve">number</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Processor</t>
-  </si>
-  <si>
-    <t xml:space="preserve">p1</t>
-  </si>
-  <si>
-    <t xml:space="preserve">p2</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ProcessorGroup</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ParentProcessor</t>
-  </si>
-  <si>
-    <t xml:space="preserve">SubsystemType</t>
-  </si>
-  <si>
-    <t xml:space="preserve">System</t>
-  </si>
-  <si>
-    <t xml:space="preserve">FunctionalOrStructural</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Accounted</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Stock</t>
-  </si>
-  <si>
-    <t xml:space="preserve">GeolocationRef</t>
-  </si>
-  <si>
-    <t xml:space="preserve">GeolocationCode</t>
-  </si>
-  <si>
-    <t xml:space="preserve">GeolocationLatLong</t>
-  </si>
-  <si>
-    <t xml:space="preserve">yes</t>
   </si>
   <si>
     <t xml:space="preserve">Interface</t>
@@ -364,7 +364,7 @@
   </sheetPr>
   <dimension ref="A1:K3"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="0" ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
       <selection pane="bottomLeft" activeCell="K3" activeCellId="0" sqref="K3"/>
@@ -464,216 +464,12 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:H5"/>
-  <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="0" ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="B3" activeCellId="0" sqref="B3"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
-  <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="10.65"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="24.17"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="14.08"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="11.07"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="1" width="11.79"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="1" width="10.65"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="1" width="12.93"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="1" width="11.79"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="9" style="0" width="9.07"/>
-  </cols>
-  <sheetData>
-    <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="B1" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="C1" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="D1" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="E1" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="F1" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="G1" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="H1" s="2" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="B2" s="4" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="C3" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="D3" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="E3" s="1" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="C4" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="D4" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="E4" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="G4" s="1" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="C5" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="D5" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="E5" s="1" t="s">
-        <v>32</v>
-      </c>
-    </row>
-  </sheetData>
-  <hyperlinks>
-    <hyperlink ref="B2" r:id="rId1" location="TheData" display="data://#TheData"/>
-  </hyperlinks>
-  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
-  <headerFooter differentFirst="false" differentOddEven="false">
-    <oddHeader/>
-    <oddFooter/>
-  </headerFooter>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <sheetPr filterMode="false">
-    <pageSetUpPr fitToPage="false"/>
-  </sheetPr>
-  <dimension ref="A1:C5"/>
+  <dimension ref="A1:M4"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="0" ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="B5" activeCellId="0" sqref="B5"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
-  <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="10.92"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="2" style="0" width="9.07"/>
-  </cols>
-  <sheetData>
-    <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="2" t="s">
-        <v>33</v>
-      </c>
-      <c r="B1" s="2" t="s">
-        <v>28</v>
-      </c>
-      <c r="C1" s="2" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="B2" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="C2" s="5" t="n">
-        <v>1.23</v>
-      </c>
-    </row>
-    <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="B3" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="C3" s="6" t="n">
-        <v>2.3</v>
-      </c>
-    </row>
-    <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="B4" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="C4" s="6" t="n">
-        <v>1.1</v>
-      </c>
-    </row>
-    <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="B5" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="C5" s="6" t="n">
-        <v>0.5</v>
-      </c>
-    </row>
-  </sheetData>
-  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
-  <headerFooter differentFirst="false" differentOddEven="false">
-    <oddHeader/>
-    <oddFooter/>
-  </headerFooter>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <sheetPr filterMode="false">
-    <pageSetUpPr fitToPage="false"/>
-  </sheetPr>
-  <dimension ref="A1:M3"/>
-  <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="0" ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+      <selection pane="bottomLeft" activeCell="B4" activeCellId="0" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -696,40 +492,40 @@
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="2" t="s">
-        <v>36</v>
+        <v>17</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>33</v>
+        <v>18</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>37</v>
+        <v>19</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>38</v>
+        <v>20</v>
       </c>
       <c r="E1" s="2" t="s">
-        <v>39</v>
+        <v>21</v>
       </c>
       <c r="F1" s="2" t="s">
-        <v>40</v>
+        <v>22</v>
       </c>
       <c r="G1" s="2" t="s">
-        <v>41</v>
+        <v>23</v>
       </c>
       <c r="H1" s="2" t="s">
-        <v>42</v>
+        <v>24</v>
       </c>
       <c r="I1" s="2" t="s">
         <v>6</v>
       </c>
       <c r="J1" s="2" t="s">
-        <v>43</v>
+        <v>25</v>
       </c>
       <c r="K1" s="2" t="s">
-        <v>44</v>
+        <v>26</v>
       </c>
       <c r="L1" s="2" t="s">
-        <v>45</v>
+        <v>27</v>
       </c>
       <c r="M1" s="2" t="s">
         <v>9</v>
@@ -737,18 +533,223 @@
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B2" s="1" t="s">
-        <v>34</v>
+        <v>28</v>
       </c>
       <c r="G2" s="1" t="s">
-        <v>46</v>
+        <v>29</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B3" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="G3" s="1" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+  </sheetData>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
+  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader/>
+    <oddFooter/>
+  </headerFooter>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1:H5"/>
+  <sheetViews>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <pane xSplit="0" ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+      <selection pane="bottomLeft" activeCell="B3" activeCellId="0" sqref="B3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <cols>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="10.65"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="24.17"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="14.08"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="11.07"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="1" width="11.79"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="1" width="10.65"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="1" width="12.93"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="1" width="11.79"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="9" style="0" width="9.07"/>
+  </cols>
+  <sheetData>
+    <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="E1" s="2" t="s">
         <v>35</v>
       </c>
-      <c r="G3" s="1" t="s">
+      <c r="F1" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="G1" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" s="2" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="B2" s="4" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="E3" s="1" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="E4" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="G4" s="1" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="D5" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="E5" s="1" t="s">
         <v>46</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="B2" r:id="rId1" location="TheData" display="data://#TheData"/>
+  </hyperlinks>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
+  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader/>
+    <oddFooter/>
+  </headerFooter>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1:C5"/>
+  <sheetViews>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <pane xSplit="0" ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+      <selection pane="bottomLeft" activeCell="B5" activeCellId="0" sqref="B5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <cols>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="10.92"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="2" style="0" width="9.07"/>
+  </cols>
+  <sheetData>
+    <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="C2" s="5" t="n">
+        <v>1.23</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="C3" s="6" t="n">
+        <v>2.3</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="C4" s="6" t="n">
+        <v>1.1</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="C5" s="6" t="n">
+        <v>0.5</v>
       </c>
     </row>
   </sheetData>
@@ -772,7 +773,7 @@
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="B1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="0" ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="B1" activeCellId="0" sqref="B1"/>
-      <selection pane="bottomLeft" activeCell="R3" activeCellId="0" sqref="R3"/>
+      <selection pane="bottomLeft" activeCell="D8" activeCellId="0" sqref="D8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -803,7 +804,7 @@
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="2" t="s">
-        <v>33</v>
+        <v>18</v>
       </c>
       <c r="B1" s="2" t="s">
         <v>1</v>
@@ -824,10 +825,10 @@
         <v>8</v>
       </c>
       <c r="H1" s="2" t="s">
-        <v>43</v>
+        <v>25</v>
       </c>
       <c r="I1" s="2" t="s">
-        <v>44</v>
+        <v>26</v>
       </c>
       <c r="J1" s="2" t="s">
         <v>49</v>

</xml_diff>

<commit_message>
Unit conversion of Interface values (InterfaceType must define a Unit)
On InterfaceCommand execution, values are converted to the reference unit of the InterfaceType. If the value is an expression, the conversion is stated symbolically: "({Value}) * {str(conv_factor)}".

To ensure InterfaceTypes have a unit, the field Unit of InterfaceType command is defined now as mandatory.

Also, bug solved regarding case sensitiveness of DatasetDef, DatasetData commands
Also, reenumeration of some tests.
</commit_message>
<xml_diff>
--- a/backend_tests/z_input_files/v2/18_dataset_expansion_2.xlsx
+++ b/backend_tests/z_input_files/v2/18_dataset_expansion_2.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="96" uniqueCount="65">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="98" uniqueCount="66">
   <si>
     <t xml:space="preserve">InterfaceTypeHierarchy</t>
   </si>
@@ -66,6 +66,9 @@
   </si>
   <si>
     <t xml:space="preserve">flow</t>
+  </si>
+  <si>
+    <t xml:space="preserve">tonnes</t>
   </si>
   <si>
     <t xml:space="preserve">0100</t>
@@ -367,10 +370,10 @@
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="0" ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="K3" activeCellId="0" sqref="K3"/>
+      <selection pane="bottomLeft" activeCell="H4" activeCellId="0" sqref="H4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="9.07421875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="20.5"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="14.35"/>
@@ -382,7 +385,6 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="1" width="8.21"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="1" width="21.63"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="1" width="11.79"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="11" style="0" width="9.07"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -430,13 +432,16 @@
       <c r="D2" s="1" t="s">
         <v>13</v>
       </c>
+      <c r="H2" s="1" t="s">
+        <v>14</v>
+      </c>
       <c r="K2" s="3" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B3" s="1" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="C3" s="1" t="s">
         <v>12</v>
@@ -444,8 +449,11 @@
       <c r="D3" s="1" t="s">
         <v>13</v>
       </c>
+      <c r="H3" s="1" t="s">
+        <v>14</v>
+      </c>
       <c r="K3" s="1" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
     </row>
   </sheetData>
@@ -472,60 +480,59 @@
       <selection pane="bottomLeft" activeCell="B4" activeCellId="0" sqref="B4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="9.07421875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="16.07"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="12.21"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="16.36"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="15.93"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="1" width="10.5"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="1" width="10.51"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="1" width="20.07"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="1" width="12.5"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="1" width="12.51"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="1" width="9.36"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="1" width="12.93"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="1" width="15.49"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="1" width="16.79"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="1" width="18.51"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="13" style="1" width="11.79"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="14" style="0" width="9.07"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="2" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="E1" s="2" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="F1" s="2" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="G1" s="2" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="H1" s="2" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="I1" s="2" t="s">
         <v>6</v>
       </c>
       <c r="J1" s="2" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="K1" s="2" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="L1" s="2" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="M1" s="2" t="s">
         <v>9</v>
@@ -533,18 +540,18 @@
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B2" s="1" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="G2" s="1" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B3" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="G3" s="1" t="s">
         <v>30</v>
-      </c>
-      <c r="G3" s="1" t="s">
-        <v>29</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
@@ -572,37 +579,36 @@
       <selection pane="bottomLeft" activeCell="B3" activeCellId="0" sqref="B3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="9.07421875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="10.65"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="10.66"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="24.17"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="14.08"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="11.07"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="1" width="11.79"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="1" width="10.65"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="1" width="10.66"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="1" width="12.93"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="1" width="11.79"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="9" style="0" width="9.07"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="2" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="E1" s="2" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="F1" s="2" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="G1" s="2" t="s">
         <v>6</v>
@@ -613,55 +619,55 @@
     </row>
     <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="1" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="B2" s="4" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="1" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="1" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="D4" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="E4" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="E4" s="1" t="s">
-        <v>41</v>
-      </c>
       <c r="G4" s="1" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="1" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
     </row>
   </sheetData>
@@ -691,29 +697,28 @@
       <selection pane="bottomLeft" activeCell="B5" activeCellId="0" sqref="B5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="9.07421875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="10.92"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="2" style="0" width="9.07"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="2" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="1" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="C2" s="5" t="n">
         <v>1.23</v>
@@ -721,10 +726,10 @@
     </row>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="1" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="C3" s="6" t="n">
         <v>2.3</v>
@@ -732,10 +737,10 @@
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="1" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="C4" s="6" t="n">
         <v>1.1</v>
@@ -743,10 +748,10 @@
     </row>
     <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="1" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="C5" s="6" t="n">
         <v>0.5</v>
@@ -776,10 +781,10 @@
       <selection pane="bottomLeft" activeCell="D8" activeCellId="0" sqref="D8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="9.07421875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="14.21"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="27.07"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="27.06"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="11.21"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="10.36"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="1" width="13.79"/>
@@ -792,25 +797,24 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="1" width="8.21"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="13" style="1" width="12.37"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="14" min="14" style="1" width="12.93"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="15" min="15" style="1" width="13.5"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="15" min="15" style="1" width="13.51"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="16" min="16" style="1" width="15.35"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="17" min="17" style="1" width="11.5"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="17" min="17" style="1" width="11.51"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="18" min="18" style="1" width="8.79"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="19" min="19" style="1" width="10.19"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="20" min="20" style="1" width="16.79"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="21" min="21" style="1" width="12.64"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="22" style="0" width="9.07"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="2" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="B1" s="2" t="s">
         <v>1</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="D1" s="2" t="s">
         <v>2</v>
@@ -819,69 +823,69 @@
         <v>3</v>
       </c>
       <c r="F1" s="2" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="G1" s="2" t="s">
         <v>8</v>
       </c>
       <c r="H1" s="2" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="I1" s="2" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="J1" s="2" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="K1" s="2" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="L1" s="2" t="s">
         <v>7</v>
       </c>
       <c r="M1" s="2" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="N1" s="2" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="O1" s="2" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="P1" s="2" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="Q1" s="2" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="R1" s="2" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="S1" s="2" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="T1" s="2" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="U1" s="2" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="1" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="K2" s="1" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="R2" s="1" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
     </row>
   </sheetData>

</xml_diff>